<commit_message>
Dynamic fee for vantai
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/KeHoachVanTaiTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/KeHoachVanTaiTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>KHÁCH HÀNG</t>
   </si>
@@ -65,9 +65,6 @@
     <t>CONT 40</t>
   </si>
   <si>
-    <t>CHI PHÍ NHÀ THẦU</t>
-  </si>
-  <si>
     <t>${detail.cusName}</t>
   </si>
   <si>
@@ -123,16 +120,41 @@
   </si>
   <si>
     <t xml:space="preserve">VẬN TẢI  </t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${details}" var="detail"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/jx:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${feeNames}" var="feeName"&gt;</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>${feeName}</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${detail.convertedFee}" var="feeVal"&gt;</t>
+  </si>
+  <si>
+    <t>${feeVal.feeVal}</t>
+  </si>
+  <si>
+    <t>Tổng cộng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +214,13 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -279,10 +308,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,22 +363,7 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,18 +375,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -649,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:T86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,106 +724,120 @@
     <col min="9" max="9" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="12" max="12" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="21.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-    </row>
-    <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="N2" s="18"/>
+    </row>
+    <row r="3" spans="1:20" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="E3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="18" t="s">
+      <c r="N3" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="6" t="s">
         <v>11</v>
       </c>
@@ -775,16 +845,19 @@
         <v>12</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -800,68 +873,86 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+    </row>
+    <row r="7" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="27" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="L7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="11" t="s">
+      <c r="M7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="N7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="12"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="B8" s="13"/>
       <c r="C8" s="15"/>
       <c r="D8" s="13"/>
@@ -869,11 +960,13 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="N8" s="13"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="37"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="15"/>
@@ -882,11 +975,15 @@
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="O9" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="P9" s="13"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="15"/>
@@ -895,11 +992,13 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
-      <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="15"/>
@@ -908,11 +1007,13 @@
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="15"/>
@@ -921,11 +1022,13 @@
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
-      <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="15"/>
@@ -934,11 +1037,13 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
-    </row>
-    <row r="14" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="15"/>
@@ -947,16 +1052,13 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="13"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
-    </row>
-    <row r="15" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+    </row>
+    <row r="15" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="15"/>
@@ -970,11 +1072,14 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="13"/>
+      <c r="N15" s="2"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+    </row>
+    <row r="16" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="15"/>
@@ -983,11 +1088,19 @@
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
-      <c r="N16" s="13"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="15"/>
@@ -996,11 +1109,13 @@
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-      <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="15"/>
@@ -1009,11 +1124,13 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="15"/>
@@ -1022,11 +1139,13 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="N19" s="13"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="15"/>
@@ -1035,11 +1154,13 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="N20" s="13"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="15"/>
@@ -1048,11 +1169,13 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
-      <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="15"/>
@@ -1061,11 +1184,13 @@
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
-      <c r="N22" s="13"/>
       <c r="O22" s="13"/>
       <c r="P22" s="13"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="15"/>
@@ -1074,11 +1199,13 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="N23" s="13"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="15"/>
@@ -1087,11 +1214,13 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="N24" s="13"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="15"/>
@@ -1100,11 +1229,13 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="N25" s="13"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="15"/>
@@ -1113,11 +1244,13 @@
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="N26" s="13"/>
       <c r="O26" s="13"/>
       <c r="P26" s="13"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="15"/>
@@ -1126,11 +1259,13 @@
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
-      <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="15"/>
@@ -1139,11 +1274,13 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
-      <c r="N28" s="13"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="15"/>
@@ -1152,11 +1289,13 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
-      <c r="N29" s="13"/>
       <c r="O29" s="13"/>
       <c r="P29" s="13"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="15"/>
@@ -1165,11 +1304,13 @@
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
-      <c r="N30" s="13"/>
       <c r="O30" s="13"/>
       <c r="P30" s="13"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="15"/>
@@ -1178,11 +1319,13 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
-      <c r="N31" s="13"/>
       <c r="O31" s="13"/>
       <c r="P31" s="13"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="15"/>
@@ -1191,11 +1334,13 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="N32" s="13"/>
       <c r="O32" s="13"/>
       <c r="P32" s="13"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="15"/>
@@ -1204,11 +1349,13 @@
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
-      <c r="N33" s="13"/>
       <c r="O33" s="13"/>
       <c r="P33" s="13"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="15"/>
@@ -1217,11 +1364,13 @@
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
-      <c r="N34" s="13"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="15"/>
@@ -1230,11 +1379,13 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
-      <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="15"/>
@@ -1243,11 +1394,13 @@
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
-      <c r="N36" s="13"/>
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="15"/>
@@ -1256,11 +1409,13 @@
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
-      <c r="N37" s="13"/>
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="15"/>
@@ -1269,11 +1424,13 @@
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
-      <c r="N38" s="13"/>
       <c r="O38" s="13"/>
       <c r="P38" s="13"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="15"/>
@@ -1282,11 +1439,13 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="15"/>
@@ -1295,11 +1454,13 @@
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="N40" s="13"/>
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="15"/>
@@ -1308,11 +1469,13 @@
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
-      <c r="N41" s="13"/>
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="15"/>
@@ -1321,11 +1484,13 @@
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
-      <c r="N42" s="13"/>
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="15"/>
@@ -1334,11 +1499,13 @@
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
-      <c r="N43" s="13"/>
       <c r="O43" s="13"/>
       <c r="P43" s="13"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="15"/>
@@ -1347,11 +1514,13 @@
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
-      <c r="N44" s="13"/>
       <c r="O44" s="13"/>
       <c r="P44" s="13"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="15"/>
@@ -1360,11 +1529,13 @@
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
-      <c r="N45" s="13"/>
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="15"/>
@@ -1373,11 +1544,13 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
-      <c r="N46" s="13"/>
       <c r="O46" s="13"/>
       <c r="P46" s="13"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="15"/>
@@ -1386,11 +1559,13 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
-      <c r="N47" s="13"/>
       <c r="O47" s="13"/>
       <c r="P47" s="13"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="15"/>
@@ -1399,11 +1574,13 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
-      <c r="N48" s="13"/>
       <c r="O48" s="13"/>
       <c r="P48" s="13"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="15"/>
@@ -1412,11 +1589,13 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
-      <c r="N49" s="13"/>
       <c r="O49" s="13"/>
       <c r="P49" s="13"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="15"/>
@@ -1425,11 +1604,13 @@
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
-      <c r="N50" s="13"/>
       <c r="O50" s="13"/>
       <c r="P50" s="13"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="15"/>
@@ -1438,11 +1619,13 @@
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
-      <c r="N51" s="13"/>
       <c r="O51" s="13"/>
       <c r="P51" s="13"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="15"/>
@@ -1451,11 +1634,13 @@
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
-      <c r="N52" s="13"/>
       <c r="O52" s="13"/>
       <c r="P52" s="13"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="13"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="15"/>
@@ -1464,11 +1649,13 @@
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
-      <c r="N53" s="13"/>
       <c r="O53" s="13"/>
       <c r="P53" s="13"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="13"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="15"/>
@@ -1477,11 +1664,13 @@
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
-      <c r="N54" s="13"/>
       <c r="O54" s="13"/>
       <c r="P54" s="13"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q54" s="13"/>
+      <c r="R54" s="13"/>
+      <c r="S54" s="13"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="15"/>
@@ -1490,11 +1679,13 @@
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
-      <c r="N55" s="13"/>
       <c r="O55" s="13"/>
       <c r="P55" s="13"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="13"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="15"/>
@@ -1503,11 +1694,13 @@
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
-      <c r="N56" s="13"/>
       <c r="O56" s="13"/>
       <c r="P56" s="13"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q56" s="13"/>
+      <c r="R56" s="13"/>
+      <c r="S56" s="13"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="15"/>
@@ -1516,11 +1709,13 @@
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
-      <c r="N57" s="13"/>
       <c r="O57" s="13"/>
       <c r="P57" s="13"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q57" s="13"/>
+      <c r="R57" s="13"/>
+      <c r="S57" s="13"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="15"/>
@@ -1529,11 +1724,13 @@
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
-      <c r="N58" s="13"/>
       <c r="O58" s="13"/>
       <c r="P58" s="13"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
+      <c r="S58" s="13"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="15"/>
@@ -1542,11 +1739,13 @@
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
-      <c r="N59" s="13"/>
       <c r="O59" s="13"/>
       <c r="P59" s="13"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q59" s="13"/>
+      <c r="R59" s="13"/>
+      <c r="S59" s="13"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="15"/>
@@ -1555,11 +1754,13 @@
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
-      <c r="N60" s="13"/>
       <c r="O60" s="13"/>
       <c r="P60" s="13"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q60" s="13"/>
+      <c r="R60" s="13"/>
+      <c r="S60" s="13"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="15"/>
@@ -1568,11 +1769,13 @@
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
-      <c r="N61" s="13"/>
       <c r="O61" s="13"/>
       <c r="P61" s="13"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q61" s="13"/>
+      <c r="R61" s="13"/>
+      <c r="S61" s="13"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="15"/>
@@ -1581,11 +1784,13 @@
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
-      <c r="N62" s="13"/>
       <c r="O62" s="13"/>
       <c r="P62" s="13"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q62" s="13"/>
+      <c r="R62" s="13"/>
+      <c r="S62" s="13"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="15"/>
@@ -1594,11 +1799,13 @@
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
-      <c r="N63" s="13"/>
       <c r="O63" s="13"/>
       <c r="P63" s="13"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q63" s="13"/>
+      <c r="R63" s="13"/>
+      <c r="S63" s="13"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="15"/>
@@ -1607,11 +1814,13 @@
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
-      <c r="N64" s="13"/>
       <c r="O64" s="13"/>
       <c r="P64" s="13"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q64" s="13"/>
+      <c r="R64" s="13"/>
+      <c r="S64" s="13"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="15"/>
@@ -1620,11 +1829,13 @@
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
-      <c r="N65" s="13"/>
       <c r="O65" s="13"/>
       <c r="P65" s="13"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q65" s="13"/>
+      <c r="R65" s="13"/>
+      <c r="S65" s="13"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="15"/>
@@ -1633,11 +1844,13 @@
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
-      <c r="N66" s="13"/>
       <c r="O66" s="13"/>
       <c r="P66" s="13"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q66" s="13"/>
+      <c r="R66" s="13"/>
+      <c r="S66" s="13"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="15"/>
@@ -1646,11 +1859,13 @@
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
-      <c r="N67" s="13"/>
       <c r="O67" s="13"/>
       <c r="P67" s="13"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q67" s="13"/>
+      <c r="R67" s="13"/>
+      <c r="S67" s="13"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="15"/>
@@ -1659,11 +1874,13 @@
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
-      <c r="N68" s="13"/>
       <c r="O68" s="13"/>
       <c r="P68" s="13"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q68" s="13"/>
+      <c r="R68" s="13"/>
+      <c r="S68" s="13"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="15"/>
@@ -1672,11 +1889,13 @@
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
-      <c r="N69" s="13"/>
       <c r="O69" s="13"/>
       <c r="P69" s="13"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q69" s="13"/>
+      <c r="R69" s="13"/>
+      <c r="S69" s="13"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="15"/>
@@ -1685,11 +1904,13 @@
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
-      <c r="N70" s="13"/>
       <c r="O70" s="13"/>
       <c r="P70" s="13"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q70" s="13"/>
+      <c r="R70" s="13"/>
+      <c r="S70" s="13"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="15"/>
@@ -1698,11 +1919,13 @@
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
-      <c r="N71" s="13"/>
       <c r="O71" s="13"/>
       <c r="P71" s="13"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="13"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="15"/>
@@ -1711,11 +1934,13 @@
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
-      <c r="N72" s="13"/>
       <c r="O72" s="13"/>
       <c r="P72" s="13"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q72" s="13"/>
+      <c r="R72" s="13"/>
+      <c r="S72" s="13"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="15"/>
@@ -1724,11 +1949,13 @@
       <c r="F73" s="13"/>
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
-      <c r="N73" s="13"/>
       <c r="O73" s="13"/>
       <c r="P73" s="13"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q73" s="13"/>
+      <c r="R73" s="13"/>
+      <c r="S73" s="13"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="15"/>
@@ -1737,11 +1964,13 @@
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
-      <c r="N74" s="13"/>
       <c r="O74" s="13"/>
       <c r="P74" s="13"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q74" s="13"/>
+      <c r="R74" s="13"/>
+      <c r="S74" s="13"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="15"/>
@@ -1750,11 +1979,13 @@
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
-      <c r="N75" s="13"/>
       <c r="O75" s="13"/>
       <c r="P75" s="13"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q75" s="13"/>
+      <c r="R75" s="13"/>
+      <c r="S75" s="13"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="15"/>
@@ -1763,11 +1994,13 @@
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
-      <c r="N76" s="13"/>
       <c r="O76" s="13"/>
       <c r="P76" s="13"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q76" s="13"/>
+      <c r="R76" s="13"/>
+      <c r="S76" s="13"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="15"/>
@@ -1776,11 +2009,13 @@
       <c r="F77" s="13"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
-      <c r="N77" s="13"/>
       <c r="O77" s="13"/>
       <c r="P77" s="13"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q77" s="13"/>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="15"/>
@@ -1789,11 +2024,13 @@
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
-      <c r="N78" s="13"/>
       <c r="O78" s="13"/>
       <c r="P78" s="13"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q78" s="13"/>
+      <c r="R78" s="13"/>
+      <c r="S78" s="13"/>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="15"/>
@@ -1802,11 +2039,13 @@
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
-      <c r="N79" s="13"/>
       <c r="O79" s="13"/>
       <c r="P79" s="13"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q79" s="13"/>
+      <c r="R79" s="13"/>
+      <c r="S79" s="13"/>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="15"/>
@@ -1815,11 +2054,13 @@
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
-      <c r="N80" s="13"/>
       <c r="O80" s="13"/>
       <c r="P80" s="13"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q80" s="13"/>
+      <c r="R80" s="13"/>
+      <c r="S80" s="13"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="15"/>
@@ -1828,11 +2069,13 @@
       <c r="F81" s="13"/>
       <c r="G81" s="13"/>
       <c r="H81" s="13"/>
-      <c r="N81" s="13"/>
       <c r="O81" s="13"/>
       <c r="P81" s="13"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q81" s="13"/>
+      <c r="R81" s="13"/>
+      <c r="S81" s="13"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="15"/>
@@ -1841,11 +2084,13 @@
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
       <c r="H82" s="13"/>
-      <c r="N82" s="13"/>
       <c r="O82" s="13"/>
       <c r="P82" s="13"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q82" s="13"/>
+      <c r="R82" s="13"/>
+      <c r="S82" s="13"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="15"/>
@@ -1854,11 +2099,13 @@
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
       <c r="H83" s="13"/>
-      <c r="N83" s="13"/>
       <c r="O83" s="13"/>
       <c r="P83" s="13"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q83" s="13"/>
+      <c r="R83" s="13"/>
+      <c r="S83" s="13"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="15"/>
@@ -1867,11 +2114,13 @@
       <c r="F84" s="13"/>
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
-      <c r="N84" s="13"/>
       <c r="O84" s="13"/>
       <c r="P84" s="13"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q84" s="13"/>
+      <c r="R84" s="13"/>
+      <c r="S84" s="13"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="15"/>
@@ -1880,16 +2129,35 @@
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
-      <c r="N85" s="13"/>
       <c r="O85" s="13"/>
       <c r="P85" s="13"/>
+      <c r="Q85" s="13"/>
+      <c r="R85" s="13"/>
+      <c r="S85" s="13"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86" s="13"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="O86" s="13"/>
+      <c r="P86" s="13"/>
+      <c r="Q86" s="13"/>
+      <c r="R86" s="13"/>
+      <c r="S86" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="18">
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
@@ -1901,6 +2169,7 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="N3:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>